<commit_message>
added code to update functionaties in sqlite database
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/output.xlsx
+++ b/SoftwareDesignUsingNLP/data/output.xlsx
@@ -38,7 +38,7 @@
     <t>['Recruit Doctors'],['Offer Plan']</t>
   </si>
   <si>
-    <t>{'hospital_department', 'Doctor_Name', 'doctor_licence_number'},{'Name_of_clinics', 'List_plan', 'Preventive_care'}</t>
+    <t>{'hospital_department', 'Doctor_Name', 'doctor_licence_number'},{'Preventive_care', 'Name_of_clinics', 'List_plan'}</t>
   </si>
   <si>
     <t xml:space="preserve"> plan the stay, shift their care to outpatient clinics</t>
@@ -47,7 +47,7 @@
     <t>['Offer Plan', 'Patient Admission'],['Patient Transfer']</t>
   </si>
   <si>
-    <t>{'Name_of_clinics', 'List_plan', 'Preventive_care'}{'Patient_age', 'Customer_phone', 'Name_of_clinics', 'Schedule_time'},{'Address_Of_clinics', 'Preventive_care', 'Policy_number'}</t>
+    <t>{'Preventive_care', 'Name_of_clinics', 'List_plan'}{'Patient_age', 'Schedule_time', 'Name_of_clinics', 'Customer_phone'},{'Address_Of_clinics', 'Policy_number', 'Preventive_care'}</t>
   </si>
   <si>
     <t xml:space="preserve"> emphasize more on preventive care to my patients</t>
@@ -56,7 +56,7 @@
     <t>['Provide reccommendation']</t>
   </si>
   <si>
-    <t>{'Address_Of_clinics', 'Preventive_care', 'Acc_type', 'Hospital_Address'}</t>
+    <t>{'Address_Of_clinics', 'Hospital_Address', 'Acc_type', 'Preventive_care'}</t>
   </si>
   <si>
     <t xml:space="preserve"> employ salaried doctors, paid per service</t>
@@ -65,7 +65,7 @@
     <t>['Recruit Doctors', 'Recruit Visiting Doctors'],['Contact doctor']</t>
   </si>
   <si>
-    <t>{'hospital_department', 'Doctor_Name', 'doctor_licence_number'}{'Coverage_policy', 'hospital_department', 'Hourly_charge_doctor', 'Doctor_Name', 'doctor_licence_number'},{'Patient_age', 'Customer_phone', 'Patient_prior_condition', 'Doctor_Name', 'Hospital_Address'}</t>
+    <t>{'hospital_department', 'Doctor_Name', 'doctor_licence_number'}{'hospital_department', 'Doctor_Name', 'doctor_licence_number', 'Hourly_charge_doctor', 'Coverage_policy'},{'Patient_age', 'Hospital_Address', 'Doctor_Name', 'Patient_prior_condition', 'Customer_phone'}</t>
   </si>
   <si>
     <t>Health Plan Member</t>
@@ -77,7 +77,7 @@
     <t>['Offer Plan']</t>
   </si>
   <si>
-    <t>{'Name_of_clinics', 'List_plan', 'Preventive_care'}</t>
+    <t>{'Preventive_care', 'Name_of_clinics', 'List_plan'}</t>
   </si>
   <si>
     <t xml:space="preserve"> find nearby doctors and hospitals</t>
@@ -86,7 +86,7 @@
     <t>['List of hospitals under plan', 'Contact doctor']</t>
   </si>
   <si>
-    <t>{'X,Y_Coordinates'}{'Patient_age', 'Customer_phone', 'Patient_prior_condition', 'Doctor_Name', 'Hospital_Address'}</t>
+    <t>{'X,Y_Coordinates'}{'Patient_age', 'Hospital_Address', 'Doctor_Name', 'Patient_prior_condition', 'Customer_phone'}</t>
   </si>
   <si>
     <t>Patient</t>
@@ -98,7 +98,7 @@
     <t>['Payment Process ']</t>
   </si>
   <si>
-    <t>{'Discharge_amount', 'Hospital_Address', 'Acc_type', 'Doctor_Name', 'Schedule_time'}</t>
+    <t>{'Discharge_amount', 'Hospital_Address', 'Doctor_Name', 'Acc_type', 'Schedule_time'}</t>
   </si>
   <si>
     <t xml:space="preserve"> see my medical reports online</t>
@@ -107,7 +107,7 @@
     <t>['Schedule visit']</t>
   </si>
   <si>
-    <t>{'Schedule_time', 'Doctor_available_time'}</t>
+    <t>{'Doctor_available_time', 'Schedule_time'}</t>
   </si>
   <si>
     <t xml:space="preserve"> see my Doctor, schedule my visit online</t>
@@ -116,7 +116,7 @@
     <t>['Schedule visit', 'Recruit Doctors'],['Recruit Visiting Doctors', 'Schedule visit']</t>
   </si>
   <si>
-    <t>{'Schedule_time', 'Doctor_available_time'}{'hospital_department', 'Doctor_Name', 'doctor_licence_number'},{'Coverage_policy', 'hospital_department', 'Hourly_charge_doctor', 'Doctor_Name', 'doctor_licence_number'}{'Schedule_time', 'Doctor_available_time'}</t>
+    <t>{'Doctor_available_time', 'Schedule_time'}{'hospital_department', 'Doctor_Name', 'doctor_licence_number'},{'hospital_department', 'Doctor_Name', 'doctor_licence_number', 'Hourly_charge_doctor', 'Coverage_policy'}{'Doctor_available_time', 'Schedule_time'}</t>
   </si>
 </sst>
 </file>

</xml_diff>